<commit_message>
test with other datas 100% hit
</commit_message>
<xml_diff>
--- a/input/input_test2.xlsx
+++ b/input/input_test2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyProjects\company-description\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F72D813-87A8-4B67-8913-BE455A43AC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA75D3AF-76A4-4B97-9D88-F5A226E98DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-828" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="384" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -27,67 +27,67 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
-    <t>SABC</t>
-  </si>
-  <si>
-    <t>Saeta TV (Canal 10)</t>
-  </si>
-  <si>
-    <t>Samaa TV</t>
-  </si>
-  <si>
-    <t>Sanoma</t>
-  </si>
-  <si>
-    <t>Saudi Broadcasting Authority (SBA)</t>
-  </si>
-  <si>
-    <t>Saudi Telecom Company (STC, Jawwy)</t>
-  </si>
-  <si>
-    <t>SBS Television</t>
-  </si>
-  <si>
-    <t>SBT</t>
-  </si>
-  <si>
-    <t>Sekom Iletisim sistemleri</t>
-  </si>
-  <si>
-    <t>Sentech</t>
-  </si>
-  <si>
-    <t>Servus TV</t>
-  </si>
-  <si>
-    <t>SES Global</t>
-  </si>
-  <si>
-    <t>Setar</t>
-  </si>
-  <si>
-    <t>Seven Network</t>
-  </si>
-  <si>
-    <t>SFR</t>
-  </si>
-  <si>
-    <t>SIC</t>
-  </si>
-  <si>
-    <t>Siemens</t>
-  </si>
-  <si>
-    <t>Sigma</t>
-  </si>
-  <si>
-    <t>Silknet</t>
-  </si>
-  <si>
-    <t>Sinclair Broadcast Group</t>
-  </si>
-  <si>
-    <t>Singtel</t>
+    <t>Turkish Radio and Television Corporation (TRT)</t>
+  </si>
+  <si>
+    <t>TV Azteca</t>
+  </si>
+  <si>
+    <t>TV Globo</t>
+  </si>
+  <si>
+    <t>TV Markiza</t>
+  </si>
+  <si>
+    <t>TV Nova (Czech Republic)</t>
+  </si>
+  <si>
+    <t>TV Prima</t>
+  </si>
+  <si>
+    <t>TV Puls</t>
+  </si>
+  <si>
+    <t>TV Visjon Norge</t>
+  </si>
+  <si>
+    <t>TV2 Denmark</t>
+  </si>
+  <si>
+    <t>TV2 Hungary</t>
+  </si>
+  <si>
+    <t>TV2 Norway</t>
+  </si>
+  <si>
+    <t>TV3 Group (All Media Baltics)</t>
+  </si>
+  <si>
+    <t>TV3 Lithuania</t>
+  </si>
+  <si>
+    <t>TV3 Network Ghana</t>
+  </si>
+  <si>
+    <t>TV4 (Sweden)</t>
+  </si>
+  <si>
+    <t>TV5 Monde</t>
+  </si>
+  <si>
+    <t>TV8 Turkey</t>
+  </si>
+  <si>
+    <t>TVN Discovery Group</t>
+  </si>
+  <si>
+    <t>tvOne Indonesia</t>
+  </si>
+  <si>
+    <t>TVP (Telewizja Polska)</t>
+  </si>
+  <si>
+    <t>TVRI (Televisi Republik Indonesia)</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
clean hp and li columns in output
</commit_message>
<xml_diff>
--- a/input/input_test2.xlsx
+++ b/input/input_test2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyProjects\company-description\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA75D3AF-76A4-4B97-9D88-F5A226E98DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D976A9BF-2F5E-4F21-989B-A120CE6519EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="384" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23016" yWindow="-96" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -27,67 +27,67 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
-    <t>Turkish Radio and Television Corporation (TRT)</t>
-  </si>
-  <si>
-    <t>TV Azteca</t>
-  </si>
-  <si>
-    <t>TV Globo</t>
-  </si>
-  <si>
-    <t>TV Markiza</t>
-  </si>
-  <si>
-    <t>TV Nova (Czech Republic)</t>
-  </si>
-  <si>
-    <t>TV Prima</t>
-  </si>
-  <si>
-    <t>TV Puls</t>
-  </si>
-  <si>
-    <t>TV Visjon Norge</t>
-  </si>
-  <si>
-    <t>TV2 Denmark</t>
-  </si>
-  <si>
-    <t>TV2 Hungary</t>
-  </si>
-  <si>
-    <t>TV2 Norway</t>
-  </si>
-  <si>
-    <t>TV3 Group (All Media Baltics)</t>
-  </si>
-  <si>
-    <t>TV3 Lithuania</t>
-  </si>
-  <si>
-    <t>TV3 Network Ghana</t>
-  </si>
-  <si>
-    <t>TV4 (Sweden)</t>
-  </si>
-  <si>
-    <t>TV5 Monde</t>
-  </si>
-  <si>
-    <t>TV8 Turkey</t>
-  </si>
-  <si>
-    <t>TVN Discovery Group</t>
-  </si>
-  <si>
-    <t>tvOne Indonesia</t>
-  </si>
-  <si>
-    <t>TVP (Telewizja Polska)</t>
-  </si>
-  <si>
-    <t>TVRI (Televisi Republik Indonesia)</t>
+    <t>Match TV</t>
+  </si>
+  <si>
+    <t>MBC (Middle East Broadcasting Center)</t>
+  </si>
+  <si>
+    <t>MBC (Munhwa Broadcasting Corporation)</t>
+  </si>
+  <si>
+    <t>MEASAT Broadcast Network Systems</t>
+  </si>
+  <si>
+    <t>Media Broadcast</t>
+  </si>
+  <si>
+    <t>Media Nusantara Citra</t>
+  </si>
+  <si>
+    <t>MediaCorp TV</t>
+  </si>
+  <si>
+    <t>Mediapro</t>
+  </si>
+  <si>
+    <t>Mediaset</t>
+  </si>
+  <si>
+    <t>Mediawan Thematics</t>
+  </si>
+  <si>
+    <t>MEGA TV Greece</t>
+  </si>
+  <si>
+    <t>Megacable (Mega movil)</t>
+  </si>
+  <si>
+    <t>Megogo</t>
+  </si>
+  <si>
+    <t>Middle East Broadcasting Center</t>
+  </si>
+  <si>
+    <t>Millicom</t>
+  </si>
+  <si>
+    <t>Mola</t>
+  </si>
+  <si>
+    <t>Movistar</t>
+  </si>
+  <si>
+    <t>MPC (Moving Pictures)</t>
+  </si>
+  <si>
+    <t>MTN</t>
+  </si>
+  <si>
+    <t>MTS (Mobile TeleSystems)</t>
+  </si>
+  <si>
+    <t>MTS (Telekom Srbija)</t>
   </si>
 </sst>
 </file>

</xml_diff>